<commit_message>
Only support conditional formatting of type 'expression'
</commit_message>
<xml_diff>
--- a/dev.xlsx
+++ b/dev.xlsx
@@ -5,7 +5,7 @@
     <workbookView tabRatio="600" windowHeight="14980" windowWidth="25600" xWindow="0" yWindow="1080"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Worksheet" sheetId="1" r:id="RcdHxt8CCTULVzmZM"/>
+    <sheet name="Test Worksheet" sheetId="1" r:id="Rzz7HMqxJYW07kSI6"/>
   </sheets>
 </workbook>
 </file>
@@ -67,7 +67,6 @@
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
       </font>
       <fill>
         <patternFill>
@@ -125,7 +124,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A10">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!!">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>NOT(ISERROR(SEARCH("!!", A1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add DxfItem from Style
</commit_message>
<xml_diff>
--- a/dev.xlsx
+++ b/dev.xlsx
@@ -5,7 +5,7 @@
     <workbookView tabRatio="600" windowHeight="14980" windowWidth="25600" xWindow="0" yWindow="1080"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Worksheet" sheetId="1" r:id="Rzz7HMqxJYW07kSI6"/>
+    <sheet name="Test Worksheet" sheetId="1" r:id="RmaCAoW9cWehVhHV0"/>
   </sheets>
 </workbook>
 </file>
@@ -36,22 +36,62 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="1">
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
+  <fonts count="5">
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF000055"/>
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFDDEEFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEEFF"/>
+        <bgColor rgb="FFDDEEFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -59,20 +99,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCFFCC"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf applyAlignment="0" applyNumberFormat="0" applyFill="0" applyFont="0" applyBorder="0" borderId="0" fillId="0" fontId="0" numFmtId="164"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyFill="0" applyFont="1" applyBorder="0" borderId="0" fillId="0" fontId="1" numFmtId="164"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyFill="0" applyFont="1" applyBorder="0" borderId="0" fillId="0" fontId="2" numFmtId="164"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyFill="0" applyFont="1" applyBorder="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyFill="0" applyFont="1" applyBorder="0" borderId="0" fillId="0" fontId="4" numFmtId="164"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyFill="1" applyFont="1" applyBorder="0" borderId="0" fillId="2" fontId="4" numFmtId="164"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyFill="1" applyFont="1" applyBorder="0" borderId="0" fillId="3" fontId="4" numFmtId="164"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyFill="1" applyFont="1" applyBorder="1" borderId="1" fillId="3" fontId="4" numFmtId="164"/>
   </cellXfs>
   <dxfs count="1">
     <dxf>
       <font>
         <b/>
+        <i/>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF000055"/>
+        <name val="Calibri"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FF00C7"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDDEEFF"/>
+          <bgColor rgb="FFDDEEFF"/>
         </patternFill>
       </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFCCFFCC"/>
+        </top>
+        <bottom style="thick">
+          <color rgb="FF000000"/>
+        </bottom>
+        <diagonal/>
+      </border>
     </dxf>
   </dxfs>
 </styleSheet>

</xml_diff>